<commit_message>
the open excel almost work, only  need to change from bing to google
</commit_message>
<xml_diff>
--- a/Contacts.xlsx
+++ b/Contacts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liorh\Google Drive\HMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elone\Downloads\תרגיל מועמד שלא עבר הכשרה - UiPath\תרגיל מועמד שלא עבר הכשרה - UiPath\Contacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508B136B-5A13-48BA-89C5-C1144D16E050}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965715D2-5F1D-402C-BAF4-5AEECBF3AAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -89,7 +89,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -433,20 +433,20 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="24.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.875" customWidth="1"/>
+    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="6" max="6" width="14.125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -482,7 +482,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -500,7 +500,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
secon task google still not working
</commit_message>
<xml_diff>
--- a/Contacts.xlsx
+++ b/Contacts.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
-  <workbookPr/>
+  <workbookPr codeName="חוברת_עבודה_זו"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elone\Downloads\תרגיל מועמד שלא עבר הכשרה - UiPath\תרגיל מועמד שלא עבר הכשרה - UiPath\Contacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965715D2-5F1D-402C-BAF4-5AEECBF3AAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F853C0B9-2754-4482-B506-83DFF4BD7186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22416" yWindow="11640" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>שם פרטי</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>טלפון בגוגל</t>
+  </si>
+  <si>
+    <t>29/01/2025 18:42</t>
   </si>
 </sst>
 </file>
@@ -428,8 +431,29 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="0" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{61A8D0DB-238A-49C8-BFB0-29EB4FE2209F}">
+  <we:reference id="wa104381695" version="1.0.10.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA104381695" version="1.0.10.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="גיליון1"/>
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
@@ -466,7 +490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -480,7 +504,9 @@
         <v>1234</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
fixed the google issue, left to work on the excle update in the close task
</commit_message>
<xml_diff>
--- a/Contacts.xlsx
+++ b/Contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elone\Downloads\תרגיל מועמד שלא עבר הכשרה - UiPath\תרגיל מועמד שלא עבר הכשרה - UiPath\Contacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F853C0B9-2754-4482-B506-83DFF4BD7186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0395EF0-C8CC-45EA-9474-17B4E6F177F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22416" yWindow="11640" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>שם פרטי</t>
   </si>
@@ -66,13 +66,7 @@
     <t>Jacob@mail.com</t>
   </si>
   <si>
-    <t>טופל ב</t>
-  </si>
-  <si>
     <t>טלפון בגוגל</t>
-  </si>
-  <si>
-    <t>29/01/2025 18:42</t>
   </si>
 </sst>
 </file>
@@ -457,7 +451,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F4" sqref="F1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -484,13 +478,11 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -504,9 +496,7 @@
         <v>1234</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
finished need only to stable the system
</commit_message>
<xml_diff>
--- a/Contacts.xlsx
+++ b/Contacts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="חוברת_עבודה_זו"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elone\Downloads\תרגיל מועמד שלא עבר הכשרה - UiPath\תרגיל מועמד שלא עבר הכשרה - UiPath\Contacts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\elons_work\uipath-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0395EF0-C8CC-45EA-9474-17B4E6F177F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3811F144-3D73-4FDA-A9A6-E45807C5BAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22416" yWindow="11640" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F1:F4"/>
+      <selection activeCell="F2" sqref="F2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixing some generic problems
</commit_message>
<xml_diff>
--- a/Contacts.xlsx
+++ b/Contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\elons_work\uipath-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3811F144-3D73-4FDA-A9A6-E45807C5BAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CD058B-3A67-4D68-8949-10D56C5148BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F8"/>
+      <selection activeCell="F5" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>